<commit_message>
Simply some code + fixed on RcRequest
</commit_message>
<xml_diff>
--- a/Diagnostic_sequences.xlsx
+++ b/Diagnostic_sequences.xlsx
@@ -572,7 +572,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0x30;0x30;0x43;0x33;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x32;0x31;0x20;0x53;0x65;0x70;0x20;0x32;0x30;0x20;0x30;0x39;0x3A;0x32;0x37;0x3A;0x35;0x37;0x20;0x32;0x30;0x32;0x32;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x46;0x5F;0x45;0x30;0x34;0x30;0x44;0x33;0x30;0x20;0x4A;0x61;0x6E;0x20;0x31;0x33;0x20;0x31;0x38;0x3A;0x34;0x34;0x3A;0x34;0x37;0x20;0x32;0x30;0x32;0x33;0x50;0x42;0x4D;0x53;0x5F;0x48;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x33;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x34;0x3A;0x35;0x33;0x3A;0x35;0x39;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x32;0x3A;0x35;0x30;0x3A;0x34;0x39;0x20;0x32;0x30;0x32;0x35;0x50;0x42;0x4D;0x53;0x5F;0x48;0x41;0x50;0x5F;0x45;0x30;0x31;0x30;0x44;0x32;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x35;0x3A;0x31;0x38;0x3A;0x33;0x32;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x32;0x3A;0x35;0x30;0x3A;0x34;0x39;0x20;0x32;0x30;0x32;0x35</t>
+          <t>0x30;0x30;0x43;0x33;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x32;0x31;0x20;0x53;0x65;0x70;0x20;0x32;0x30;0x20;0x30;0x39;0x3A;0x32;0x37;0x3A;0x35;0x37;0x20;0x32;0x30;0x32;0x32;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x46;0x5F;0x45;0x30;0x34;0x30;0x44;0x33;0x30;0x20;0x4A;0x61;0x6E;0x20;0x31;0x33;0x20;0x31;0x38;0x3A;0x34;0x34;0x3A;0x34;0x37;0x20;0x32;0x30;0x32;0x33;0x50;0x42;0x4D;0x53;0x5F;0x48;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x33;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x34;0x3A;0x35;0x33;0x3A;0x35;0x39;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x34;0x3A;0x35;0x37;0x3A;0x32;0x34;0x20;0x32;0x30;0x32;0x35;0x50;0x42;0x4D;0x53;0x5F;0x48;0x41;0x50;0x5F;0x45;0x30;0x31;0x30;0x44;0x32;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x35;0x3A;0x31;0x38;0x3A;0x33;0x32;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x34;0x3A;0x35;0x37;0x3A;0x32;0x34;0x20;0x32;0x30;0x32;0x35</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -1018,7 +1018,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0x30;0x30;0x43;0x33;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x32;0x31;0x20;0x53;0x65;0x70;0x20;0x32;0x30;0x20;0x30;0x39;0x3A;0x32;0x37;0x3A;0x35;0x37;0x20;0x32;0x30;0x32;0x32;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x46;0x5F;0x45;0x30;0x34;0x30;0x44;0x33;0x30;0x20;0x4A;0x61;0x6E;0x20;0x31;0x33;0x20;0x31;0x38;0x3A;0x34;0x34;0x3A;0x34;0x37;0x20;0x32;0x30;0x32;0x33;0x50;0x42;0x4D;0x53;0x5F;0x48;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x33;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x34;0x3A;0x35;0x33;0x3A;0x35;0x39;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x32;0x3A;0x35;0x30;0x3A;0x34;0x39;0x20;0x32;0x30;0x32;0x35;0x50;0x42;0x4D;0x53;0x5F;0x48;0x41;0x50;0x5F;0x45;0x30;0x31;0x30;0x44;0x32;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x35;0x3A;0x31;0x38;0x3A;0x33;0x32;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x32;0x3A;0x35;0x30;0x3A;0x34;0x39;0x20;0x32;0x30;0x32;0x35</t>
+          <t>0x30;0x30;0x43;0x33;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x32;0x31;0x20;0x53;0x65;0x70;0x20;0x32;0x30;0x20;0x30;0x39;0x3A;0x32;0x37;0x3A;0x35;0x37;0x20;0x32;0x30;0x32;0x32;0x50;0x42;0x4D;0x53;0x5F;0x4D;0x42;0x46;0x5F;0x45;0x30;0x34;0x30;0x44;0x33;0x30;0x20;0x4A;0x61;0x6E;0x20;0x31;0x33;0x20;0x31;0x38;0x3A;0x34;0x34;0x3A;0x34;0x37;0x20;0x32;0x30;0x32;0x33;0x50;0x42;0x4D;0x53;0x5F;0x48;0x42;0x4D;0x5F;0x45;0x30;0x32;0x30;0x44;0x33;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x34;0x3A;0x35;0x33;0x3A;0x35;0x39;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x34;0x3A;0x35;0x37;0x3A;0x32;0x34;0x20;0x32;0x30;0x32;0x35;0x50;0x42;0x4D;0x53;0x5F;0x48;0x41;0x50;0x5F;0x45;0x30;0x31;0x30;0x44;0x32;0x30;0x20;0x53;0x65;0x70;0x20;0x20;0x37;0x20;0x31;0x35;0x3A;0x31;0x38;0x3A;0x33;0x32;0x20;0x32;0x30;0x32;0x32;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x00;0x54;0x42;0x4D;0x55;0x5F;0x4D;0x41;0x49;0x4E;0x5F;0x76;0x39;0x2E;0x39;0x2E;0x31;0x20;0x4D;0x61;0x72;0x20;0x32;0x34;0x20;0x31;0x34;0x3A;0x35;0x37;0x3A;0x32;0x34;0x20;0x32;0x30;0x32;0x35</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">

</xml_diff>